<commit_message>
final results, but analysis continuing
</commit_message>
<xml_diff>
--- a/results/BINARY_POOL/Linezolid.xlsx
+++ b/results/BINARY_POOL/Linezolid.xlsx
@@ -1197,7 +1197,7 @@
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>Uncertain</t>
+          <t>Probable Assoc w R</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr"/>
@@ -28518,7 +28518,7 @@
       </c>
       <c r="AN7" t="inlineStr">
         <is>
-          <t>Uncertain</t>
+          <t>Probable Assoc w R</t>
         </is>
       </c>
       <c r="AO7" t="inlineStr"/>

</xml_diff>